<commit_message>
Begining to update for arrays and lists
</commit_message>
<xml_diff>
--- a/NewAutograder/assignments.xlsx
+++ b/NewAutograder/assignments.xlsx
@@ -14,6 +14,8 @@
     <sheet name="Assignment 5 - Plotting" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Assignment 6 - Strings" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Assignment 7 - While Loops" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Assignment 8 - Lists and Arrays" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Assignment 9 - Solution Comparison" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1553,4 +1555,296 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>test_type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>variable_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>expected_list</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>order_matters</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>tolerance</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>expected_array</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>expected_value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>list_equals</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>my_list</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[1, 2, 3, 4, 5]</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>List should equal [1, 2, 3, 4, 5] with order</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>list_equals</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sorted_numbers</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[10, 20, 30, 40]</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Should contain [10, 20, 30, 40] (order not important)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>array_equals</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>data_array</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>NumPy array should match expected values</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>[1.5, 2.5, 3.5, 4.5]</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>variable_type</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>my_list</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>my_list should be a list</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>list</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>test_type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>solution_file</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>variables_to_compare</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>tolerance</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>function_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>compare_solution</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>solutions/assignment9_solution.py</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>result, sum_total, average</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Compare key variables with solution file</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>function_exists</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Function process_data should exist</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>process_data</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>for_loop_used</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Should use a for loop</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>